<commit_message>
Modify output file to human understandable format
</commit_message>
<xml_diff>
--- a/localOutput.xlsx
+++ b/localOutput.xlsx
@@ -428,10 +428,10 @@
         <v>650.0</v>
       </c>
       <c r="N5" t="n">
-        <v>-1.2400000000000002</v>
+        <v>-0.6200000000000001</v>
       </c>
       <c r="O5" t="n">
-        <v>0.0</v>
+        <v>-0.6200000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>650.0</v>
       </c>
       <c r="N6" t="n">
-        <v>-1.2400000000000002</v>
+        <v>-0.6200000000000001</v>
       </c>
       <c r="O6" t="n">
         <v>-0.6200000000000001</v>
@@ -522,7 +522,7 @@
         <v>650.0</v>
       </c>
       <c r="N7" t="n">
-        <v>-1.2400000000000002</v>
+        <v>-0.6200000000000001</v>
       </c>
       <c r="O7" t="n">
         <v>-0.6200000000000001</v>
@@ -569,7 +569,7 @@
         <v>650.0</v>
       </c>
       <c r="N8" t="n">
-        <v>-1.2400000000000002</v>
+        <v>-0.6200000000000001</v>
       </c>
       <c r="O8" t="n">
         <v>-0.6200000000000001</v>
@@ -1133,10 +1133,10 @@
         <v>945.0</v>
       </c>
       <c r="N20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O20" t="n">
         <v>-0.34999999999999964</v>
-      </c>
-      <c r="O20" t="n">
-        <v>0.0</v>
       </c>
     </row>
     <row r="21">
@@ -1180,10 +1180,10 @@
         <v>945.0</v>
       </c>
       <c r="N21" t="n">
-        <v>-0.14000000000000057</v>
+        <v>0.0</v>
       </c>
       <c r="O21" t="n">
-        <v>-0.0699999999999994</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22">
@@ -1368,10 +1368,10 @@
         <v>725.0</v>
       </c>
       <c r="N25" t="n">
-        <v>-0.3300000000000005</v>
+        <v>-0.31000000000000005</v>
       </c>
       <c r="O25" t="n">
-        <v>0.0</v>
+        <v>-0.020000000000000462</v>
       </c>
     </row>
     <row r="26">
@@ -1415,10 +1415,10 @@
         <v>765.0</v>
       </c>
       <c r="N26" t="n">
-        <v>-0.5699999999999998</v>
+        <v>-0.2599999999999998</v>
       </c>
       <c r="O26" t="n">
-        <v>-0.020000000000000462</v>
+        <v>-0.31000000000000005</v>
       </c>
     </row>
     <row r="27">
@@ -1462,7 +1462,7 @@
         <v>765.0</v>
       </c>
       <c r="N27" t="n">
-        <v>-0.21999999999999975</v>
+        <v>0.0</v>
       </c>
       <c r="O27" t="n">
         <v>0.0</v>
@@ -1697,10 +1697,10 @@
         <v>0.0</v>
       </c>
       <c r="N32" t="n">
-        <v>-0.9700000000000002</v>
+        <v>-0.17999999999999994</v>
       </c>
       <c r="O32" t="n">
-        <v>0.0</v>
+        <v>-0.7900000000000001</v>
       </c>
     </row>
     <row r="33">
@@ -1744,10 +1744,10 @@
         <v>610.0</v>
       </c>
       <c r="N33" t="n">
-        <v>-2.69</v>
+        <v>-2.51</v>
       </c>
       <c r="O33" t="n">
-        <v>-0.7900000000000001</v>
+        <v>-0.17999999999999994</v>
       </c>
     </row>
     <row r="34">
@@ -1791,10 +1791,10 @@
         <v>810.0</v>
       </c>
       <c r="N34" t="n">
-        <v>-2.84</v>
+        <v>-0.33000000000000007</v>
       </c>
       <c r="O34" t="n">
-        <v>-0.04000000000000026</v>
+        <v>-2.37</v>
       </c>
     </row>
     <row r="35">
@@ -1838,10 +1838,10 @@
         <v>810.0</v>
       </c>
       <c r="N35" t="n">
-        <v>-0.33000000000000007</v>
+        <v>0.0</v>
       </c>
       <c r="O35" t="n">
-        <v>-0.5399999999999996</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36">
@@ -2543,10 +2543,10 @@
         <v>945.0</v>
       </c>
       <c r="N50" t="n">
-        <v>-0.3500000000000006</v>
+        <v>-0.21999999999999975</v>
       </c>
       <c r="O50" t="n">
-        <v>0.0</v>
+        <v>-0.13000000000000078</v>
       </c>
     </row>
     <row r="51">
@@ -2778,10 +2778,10 @@
         <v>0.0</v>
       </c>
       <c r="N55" t="n">
-        <v>-1.98</v>
+        <v>-1.23</v>
       </c>
       <c r="O55" t="n">
-        <v>0.0</v>
+        <v>-0.75</v>
       </c>
     </row>
     <row r="56">
@@ -2825,10 +2825,10 @@
         <v>0.0</v>
       </c>
       <c r="N56" t="n">
-        <v>-2.23</v>
+        <v>-1.0</v>
       </c>
       <c r="O56" t="n">
-        <v>-0.75</v>
+        <v>-1.23</v>
       </c>
     </row>
     <row r="57">
@@ -2872,10 +2872,10 @@
         <v>870.0</v>
       </c>
       <c r="N57" t="n">
-        <v>-3.94</v>
+        <v>-2.94</v>
       </c>
       <c r="O57" t="n">
-        <v>-0.8199999999999998</v>
+        <v>-0.5899999999999999</v>
       </c>
     </row>
     <row r="58">
@@ -2919,10 +2919,10 @@
         <v>1070.0</v>
       </c>
       <c r="N58" t="n">
-        <v>-2.94</v>
+        <v>0.0</v>
       </c>
       <c r="O58" t="n">
-        <v>-0.75</v>
+        <v>-2.69</v>
       </c>
     </row>
     <row r="59">
@@ -2969,7 +2969,7 @@
         <v>0.0</v>
       </c>
       <c r="O59" t="n">
-        <v>-2.76</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="60">
@@ -3342,10 +3342,10 @@
         <v>1385.0</v>
       </c>
       <c r="N67" t="n">
-        <v>-0.1299999999999999</v>
+        <v>-0.040000000000000036</v>
       </c>
       <c r="O67" t="n">
-        <v>0.0</v>
+        <v>-0.08999999999999986</v>
       </c>
     </row>
     <row r="68">
@@ -3906,10 +3906,10 @@
         <v>0.0</v>
       </c>
       <c r="N79" t="n">
-        <v>-1.33</v>
+        <v>-1.0</v>
       </c>
       <c r="O79" t="n">
-        <v>0.0</v>
+        <v>-0.33000000000000007</v>
       </c>
     </row>
     <row r="80">
@@ -3953,10 +3953,10 @@
         <v>0.0</v>
       </c>
       <c r="N80" t="n">
-        <v>-1.87</v>
+        <v>-0.8700000000000003</v>
       </c>
       <c r="O80" t="n">
-        <v>-0.33000000000000007</v>
+        <v>-0.9999999999999999</v>
       </c>
     </row>
     <row r="81">
@@ -4000,7 +4000,7 @@
         <v>870.0</v>
       </c>
       <c r="N81" t="n">
-        <v>-3.43</v>
+        <v>-2.43</v>
       </c>
       <c r="O81" t="n">
         <v>0.0</v>
@@ -4047,10 +4047,10 @@
         <v>870.0</v>
       </c>
       <c r="N82" t="n">
-        <v>-2.5699999999999994</v>
+        <v>0.0</v>
       </c>
       <c r="O82" t="n">
-        <v>-0.8600000000000001</v>
+        <v>-2.43</v>
       </c>
     </row>
     <row r="83">
@@ -4094,10 +4094,10 @@
         <v>870.0</v>
       </c>
       <c r="N83" t="n">
-        <v>-0.10999999999999988</v>
+        <v>-0.11000000000000032</v>
       </c>
       <c r="O83" t="n">
-        <v>-2.57</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="84">
@@ -4141,10 +4141,10 @@
         <v>1070.0</v>
       </c>
       <c r="N84" t="n">
-        <v>-0.14000000000000012</v>
+        <v>-0.03000000000000025</v>
       </c>
       <c r="O84" t="n">
-        <v>0.0</v>
+        <v>-0.11000000000000032</v>
       </c>
     </row>
     <row r="85">
@@ -4188,10 +4188,10 @@
         <v>1260.0</v>
       </c>
       <c r="N85" t="n">
-        <v>-0.3900000000000001</v>
+        <v>-0.36000000000000026</v>
       </c>
       <c r="O85" t="n">
-        <v>-0.11000000000000032</v>
+        <v>-0.03000000000000025</v>
       </c>
     </row>
     <row r="86">
@@ -4752,10 +4752,10 @@
         <v>810.0</v>
       </c>
       <c r="N97" t="n">
-        <v>-0.40000000000000036</v>
+        <v>-0.3200000000000003</v>
       </c>
       <c r="O97" t="n">
-        <v>0.0</v>
+        <v>-0.08000000000000007</v>
       </c>
     </row>
     <row r="98">
@@ -4799,10 +4799,10 @@
         <v>810.0</v>
       </c>
       <c r="N98" t="n">
-        <v>-0.40000000000000036</v>
+        <v>-0.08000000000000007</v>
       </c>
       <c r="O98" t="n">
-        <v>-0.08000000000000007</v>
+        <v>-0.3200000000000003</v>
       </c>
     </row>
     <row r="99">
@@ -5081,10 +5081,10 @@
         <v>0.0</v>
       </c>
       <c r="N104" t="n">
-        <v>-1.8299999999999996</v>
+        <v>-0.86</v>
       </c>
       <c r="O104" t="n">
-        <v>0.0</v>
+        <v>-0.9699999999999999</v>
       </c>
     </row>
     <row r="105">
@@ -5128,10 +5128,10 @@
         <v>850.0</v>
       </c>
       <c r="N105" t="n">
-        <v>-3.4</v>
+        <v>-2.48</v>
       </c>
       <c r="O105" t="n">
-        <v>-0.049999999999999926</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="106">
@@ -5175,10 +5175,10 @@
         <v>850.0</v>
       </c>
       <c r="N106" t="n">
-        <v>-2.54</v>
+        <v>0.0</v>
       </c>
       <c r="O106" t="n">
-        <v>-0.86</v>
+        <v>-2.48</v>
       </c>
     </row>
     <row r="107">
@@ -5222,10 +5222,10 @@
         <v>1050.0</v>
       </c>
       <c r="N107" t="n">
-        <v>-0.17999999999999972</v>
+        <v>0.0</v>
       </c>
       <c r="O107" t="n">
-        <v>-1.6399999999999997</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="108">
@@ -5269,7 +5269,7 @@
         <v>1070.0</v>
       </c>
       <c r="N108" t="n">
-        <v>-0.17999999999999972</v>
+        <v>0.0</v>
       </c>
       <c r="O108" t="n">
         <v>0.0</v>
@@ -5316,10 +5316,10 @@
         <v>1500.0</v>
       </c>
       <c r="N109" t="n">
-        <v>-0.4299999999999997</v>
+        <v>-0.3200000000000003</v>
       </c>
       <c r="O109" t="n">
-        <v>-0.07000000000000028</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="110">
@@ -5880,10 +5880,10 @@
         <v>830.0</v>
       </c>
       <c r="N121" t="n">
-        <v>-0.39000000000000057</v>
+        <v>-0.3100000000000005</v>
       </c>
       <c r="O121" t="n">
-        <v>0.0</v>
+        <v>-0.08000000000000007</v>
       </c>
     </row>
     <row r="122">
@@ -6209,10 +6209,10 @@
         <v>0.0</v>
       </c>
       <c r="N128" t="n">
-        <v>-0.82</v>
+        <v>-0.51</v>
       </c>
       <c r="O128" t="n">
-        <v>0.0</v>
+        <v>-0.30999999999999994</v>
       </c>
     </row>
     <row r="129">
@@ -6256,7 +6256,7 @@
         <v>525.0</v>
       </c>
       <c r="N129" t="n">
-        <v>-1.7400000000000002</v>
+        <v>-1.4300000000000004</v>
       </c>
       <c r="O129" t="n">
         <v>0.0</v>
@@ -6303,10 +6303,10 @@
         <v>525.0</v>
       </c>
       <c r="N130" t="n">
-        <v>-1.5</v>
+        <v>0.0</v>
       </c>
       <c r="O130" t="n">
-        <v>-0.24000000000000032</v>
+        <v>-1.4300000000000004</v>
       </c>
     </row>
     <row r="131">
@@ -6353,7 +6353,7 @@
         <v>-0.06999999999999984</v>
       </c>
       <c r="O131" t="n">
-        <v>-1.5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="132">
@@ -6867,10 +6867,10 @@
         <v>640.0</v>
       </c>
       <c r="N142" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O142" t="n">
         <v>-0.1499999999999999</v>
-      </c>
-      <c r="O142" t="n">
-        <v>0.0</v>
       </c>
     </row>
     <row r="143">
@@ -6917,7 +6917,7 @@
         <v>-0.22000000000000022</v>
       </c>
       <c r="O143" t="n">
-        <v>-0.1499999999999999</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="144">
@@ -6961,10 +6961,10 @@
         <v>600.0</v>
       </c>
       <c r="N144" t="n">
-        <v>-0.37999999999999984</v>
+        <v>-0.1599999999999997</v>
       </c>
       <c r="O144" t="n">
-        <v>0.0</v>
+        <v>-0.22000000000000022</v>
       </c>
     </row>
     <row r="145">
@@ -7008,7 +7008,7 @@
         <v>600.0</v>
       </c>
       <c r="N145" t="n">
-        <v>-0.31999999999999984</v>
+        <v>-0.09999999999999964</v>
       </c>
       <c r="O145" t="n">
         <v>0.0</v>
@@ -7290,10 +7290,10 @@
         <v>0.0</v>
       </c>
       <c r="N151" t="n">
-        <v>-0.4800000000000001</v>
+        <v>-0.2</v>
       </c>
       <c r="O151" t="n">
-        <v>0.0</v>
+        <v>-0.28</v>
       </c>
     </row>
     <row r="152">
@@ -7337,10 +7337,10 @@
         <v>0.0</v>
       </c>
       <c r="N152" t="n">
-        <v>-0.30000000000000004</v>
+        <v>-0.10000000000000003</v>
       </c>
       <c r="O152" t="n">
-        <v>-0.28</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="153">
@@ -7384,7 +7384,7 @@
         <v>200.0</v>
       </c>
       <c r="N153" t="n">
-        <v>-0.12000000000000002</v>
+        <v>0.0</v>
       </c>
       <c r="O153" t="n">
         <v>0.0</v>
@@ -8168,7 +8168,7 @@
         <v>25</v>
       </c>
       <c r="B174" t="n">
-        <v>57.07999999999999</v>
+        <v>29.879999999999992</v>
       </c>
     </row>
     <row r="175">
@@ -8176,7 +8176,7 @@
         <v>26</v>
       </c>
       <c r="B175" t="n">
-        <v>17.14</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="176">

</xml_diff>